<commit_message>
A2 - Connected the application to Spiros database, tested, and all is working!
</commit_message>
<xml_diff>
--- a/Assignment_2/Assignment2_TestPlan/TestPlan.xlsx
+++ b/Assignment_2/Assignment2_TestPlan/TestPlan.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthew Grayum\Dropbox\MATT\SPRING 2018\MIS 124\Assignment2_TestPlan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthew Grayum\source\repos\MIS124\Assignment_2\Assignment2_TestPlan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64EC9E0A-E9E0-4A37-AE22-0A8C06226849}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFD108A0-EAFF-43D1-8AA7-640C405D5787}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14538" windowHeight="5886" xr2:uid="{00780A6C-A250-4A92-AB6B-E19A2F099472}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="52">
   <si>
     <t>Test Case</t>
   </si>
@@ -242,6 +242,15 @@
   </si>
   <si>
     <t>Each test case was conducted to ensure that the application performed as expected</t>
+  </si>
+  <si>
+    <t>An error message will display, the DetailsView will remain in edit mode, and the record will not be updated</t>
+  </si>
+  <si>
+    <t>DetailsView edit mode: User enters an incorrectly formatted zip code</t>
+  </si>
+  <si>
+    <t>DetailsView edit mode: User enters an invalid State abbreviation</t>
   </si>
 </sst>
 </file>
@@ -516,7 +525,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -527,6 +536,63 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -536,15 +602,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -557,53 +614,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -919,10 +934,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A38FA25-0A53-450C-ACF4-C7A0D5762E98}">
-  <dimension ref="A1:C36"/>
+  <dimension ref="A1:C38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -933,315 +948,337 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="7" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="7" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="7" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="7" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="8" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
+      <c r="B7" s="29"/>
+      <c r="C7" s="29"/>
     </row>
     <row r="8" spans="1:3" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="C8" s="1"/>
     </row>
     <row r="9" spans="1:3" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="11"/>
-      <c r="C9" s="12"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="28"/>
     </row>
     <row r="10" spans="1:3" s="2" customFormat="1" ht="29.1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="6" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="72" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="17" t="s">
+      <c r="A11" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="20" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="57.9" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A12" s="18" t="s">
+      <c r="C11" s="13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="B12" s="21" t="s">
+      <c r="B12" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="22" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
-    <row r="14" spans="1:3" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A14" s="4" t="s">
+      <c r="C12" s="20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" s="30" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" s="20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="29.1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A14" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
+    <row r="16" spans="1:3" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A16" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="6"/>
-    </row>
-    <row r="15" spans="1:3" s="2" customFormat="1" ht="29.1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A15" s="7" t="s">
+      <c r="B16" s="24"/>
+      <c r="C16" s="25"/>
+    </row>
+    <row r="17" spans="1:3" s="2" customFormat="1" ht="29.1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A17" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B17" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C17" s="6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="24" t="s">
+    <row r="18" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B16" s="25" t="s">
+      <c r="B18" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="20" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="26" t="s">
+      <c r="C18" s="13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="23" t="s">
+      <c r="B19" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="C17" s="27" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="26" t="s">
+      <c r="C19" s="20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="23" t="s">
+      <c r="B20" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="C18" s="27" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="26" t="s">
+      <c r="C20" s="20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="B19" s="23" t="s">
+      <c r="B21" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="C19" s="27" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="26" t="s">
+      <c r="C21" s="20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="B20" s="23" t="s">
+      <c r="B22" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="C20" s="27" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="26"/>
-      <c r="B21" s="23"/>
-      <c r="C21" s="27"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" s="26" t="s">
+      <c r="C22" s="20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" s="19"/>
+      <c r="B23" s="16"/>
+      <c r="C23" s="20"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B22" s="23" t="s">
+      <c r="B24" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="C22" s="27" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="26" t="s">
+      <c r="C24" s="20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="B23" s="23" t="s">
+      <c r="B25" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="27" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" s="26" t="s">
+      <c r="C25" s="20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="B24" s="23" t="s">
+      <c r="B26" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="C24" s="27" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="57.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25" s="26" t="s">
+      <c r="C26" s="20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="B25" s="23" t="s">
+      <c r="B27" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="C25" s="27" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" s="26" t="s">
+      <c r="C27" s="20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B26" s="23" t="s">
+      <c r="B28" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C26" s="27" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" s="26" t="s">
+      <c r="C28" s="20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="B27" s="23" t="s">
+      <c r="B29" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="27" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28" s="26" t="s">
+      <c r="C29" s="20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="B28" s="23" t="s">
+      <c r="B30" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C28" s="27" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A29" s="26" t="s">
+      <c r="C30" s="20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B29" s="23" t="s">
+      <c r="B31" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="C29" s="27" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="43.5" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A30" s="28" t="s">
+      <c r="C31" s="20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="43.5" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A32" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="B30" s="29" t="s">
+      <c r="B32" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="C30" s="22" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
-    <row r="32" spans="1:3" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A32" s="4" t="s">
+      <c r="C32" s="15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
+    <row r="34" spans="1:3" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A34" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="B32" s="5"/>
-      <c r="C32" s="6"/>
-    </row>
-    <row r="33" spans="1:3" s="2" customFormat="1" ht="29.1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A33" s="7" t="s">
+      <c r="B34" s="24"/>
+      <c r="C34" s="25"/>
+    </row>
+    <row r="35" spans="1:3" s="2" customFormat="1" ht="29.1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A35" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B33" s="16" t="s">
+      <c r="B35" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C33" s="9" t="s">
+      <c r="C35" s="6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="129.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A34" s="24" t="s">
+    <row r="36" spans="1:3" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="B34" s="25" t="s">
+      <c r="B36" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="C34" s="20" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="129.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A35" s="26" t="s">
+      <c r="C36" s="13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="B35" s="23" t="s">
+      <c r="B37" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="C35" s="27" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="29.1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A36" s="28" t="s">
+      <c r="C37" s="20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="29.1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A38" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="B36" s="29" t="s">
+      <c r="B38" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="C36" s="22" t="s">
+      <c r="C38" s="15" t="s">
         <v>42</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="A16:C16"/>
     <mergeCell ref="A9:C9"/>
-    <mergeCell ref="A32:C32"/>
+    <mergeCell ref="A34:C34"/>
     <mergeCell ref="A7:C7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
A2 Final Commit ? (are we ever truly done?)
</commit_message>
<xml_diff>
--- a/Assignment_2/Assignment2_TestPlan/TestPlan.xlsx
+++ b/Assignment_2/Assignment2_TestPlan/TestPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthew Grayum\source\repos\MIS124\Assignment_2\Assignment2_TestPlan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFD108A0-EAFF-43D1-8AA7-640C405D5787}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65EBA726-3BCE-40F6-8E47-71682CAA5D5D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14538" windowHeight="5886" xr2:uid="{00780A6C-A250-4A92-AB6B-E19A2F099472}"/>
   </bookViews>
@@ -105,43 +105,100 @@
     <t>Result Page</t>
   </si>
   <si>
+    <t>User clicks the 'Back' button</t>
+  </si>
+  <si>
+    <t>User is redirected back to the Display Tax Return page and the same Tax Payer and Tax Return are displayed</t>
+  </si>
+  <si>
+    <t>Error message will display next to empty control and user will not be allowed to proceed until corrected</t>
+  </si>
+  <si>
+    <t>Error message will display next to the control and user will not be allowed to proceed until corrected</t>
+  </si>
+  <si>
+    <t>Error message will display next to the control that is in error and user will not be allowed to proceed until corrected</t>
+  </si>
+  <si>
+    <t>User sets IndividualOrJoint list box to 'Joint', and there IS a Joint Tax Payer in the database associated with the selected tax payer</t>
+  </si>
+  <si>
+    <t>User sets IndividualOrJoint list box to 'Joint', and there IS NOT a Joint Tax Payer in the database associated with the selected tax payer</t>
+  </si>
+  <si>
+    <t>User attempts to add/update tax return with Wages + Taxable Interest + Unemployement Compensation of over $100,000</t>
+  </si>
+  <si>
+    <t>User edits information in the Tax Payer controls at the top of the page</t>
+  </si>
+  <si>
+    <t>When the Update, Save, or Calculate buttons are clicked, the Tax Payer data on the form will be used to update the Tax Payer in the database. This way, any edits will be captured</t>
+  </si>
+  <si>
+    <t>User selects a tax year for which there is NOT a tax return in the database</t>
+  </si>
+  <si>
+    <t>User enters a tax year for which there IS a record in the database</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Matthew Grayum</t>
+  </si>
+  <si>
+    <t>Professor Spiros Velianitis</t>
+  </si>
+  <si>
+    <t>Due Date: April 23, 2018</t>
+  </si>
+  <si>
+    <t>MIS 124 - Assignment 2</t>
+  </si>
+  <si>
+    <t>California State University Sacramento</t>
+  </si>
+  <si>
+    <t>Each test case was conducted to ensure that the application performed as expected</t>
+  </si>
+  <si>
+    <t>An error message will display, the DetailsView will remain in edit mode, and the record will not be updated</t>
+  </si>
+  <si>
+    <t>DetailsView edit mode: User enters an incorrectly formatted zip code</t>
+  </si>
+  <si>
+    <t>DetailsView edit mode: User enters an invalid State abbreviation</t>
+  </si>
+  <si>
     <t>User enters Tax Return data as follows:
-*                                      Filing Independently
-* Wages =                                            $ 39,561.21
-* Taxable Interest =                                      53.42
-* Unemployment =                                         0.00
-*                              None claimed as Dependent
-* Withholding =                                       4,215.33
-* Earned Income Credit =                              0.00
-* Nontaxable combat pay =                  5,003.64</t>
+*                                                                    Married filing jointly
+* Wages =                                                                    $ 95,000.00
+* Taxable Interest =                                                         1,242.16
+* Unemployment =                                                         1,115.53
+*                                                   Spouse claimed as Dependent
+* Withholding =                                                             10,628.38
+* Earned Income Credit =                                                      0.00
+* Nontaxable combat pay =                                                  0.00</t>
+  </si>
+  <si>
+    <t>User enters Tax Return data as follows:
+*                                                                  Filing Independently
+* Wages =                                                                  $ 39,561.21
+* Taxable Interest =                                                            53.42
+* Unemployment =                                                              0.00
+*                                                   None claimed as Dependent
+* Withholding =                                                            4,215.33
+* Earned Income Credit =                                                   0.00
+* Nontaxable combat pay =                                        5,003.64</t>
   </si>
   <si>
     <r>
-      <t xml:space="preserve">* Adjusted Grs Income =  $ 39,614.63
-* Standard Deduction =       10,400.00
-* Taxable Income =               29,214.63
-* Total Payments/Credits =   4,215.33
-* Tax =                                        3,918.00
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>* Amount of Refund =                297.33</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">* Adjusted Grs Income =  $ 97,357.69
-* Standard Deduction =       16,750.00
-* Taxable Income =               80,607.69
-* Total Payments/Credits = 10,628.38
-* Tax =                                      11,634.00
+      <t xml:space="preserve">* Adjusted Grs Income =                                     $ 97,357.69
+* Standard Deduction =                                          16,750.00
+* Taxable Income =                                                  80,607.69
+* Total Payments/Credits =                                    10,628.38
+* Tax =                                                                       11,634.00
 </t>
     </r>
     <r>
@@ -162,7 +219,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">                   </t>
+      <t xml:space="preserve">                                                     </t>
     </r>
     <r>
       <rPr>
@@ -176,81 +233,24 @@
     </r>
   </si>
   <si>
-    <t>User clicks the 'Back' button</t>
-  </si>
-  <si>
-    <t>User is redirected back to the Display Tax Return page and the same Tax Payer and Tax Return are displayed</t>
-  </si>
-  <si>
-    <t>Error message will display next to empty control and user will not be allowed to proceed until corrected</t>
-  </si>
-  <si>
-    <t>Error message will display next to the control and user will not be allowed to proceed until corrected</t>
-  </si>
-  <si>
-    <t>Error message will display next to the control that is in error and user will not be allowed to proceed until corrected</t>
-  </si>
-  <si>
-    <t>User sets IndividualOrJoint list box to 'Joint', and there IS a Joint Tax Payer in the database associated with the selected tax payer</t>
-  </si>
-  <si>
-    <t>User sets IndividualOrJoint list box to 'Joint', and there IS NOT a Joint Tax Payer in the database associated with the selected tax payer</t>
-  </si>
-  <si>
-    <t>User attempts to add/update tax return with Wages + Taxable Interest + Unemployement Compensation of over $100,000</t>
-  </si>
-  <si>
-    <t>User edits information in the Tax Payer controls at the top of the page</t>
-  </si>
-  <si>
-    <t>When the Update, Save, or Calculate buttons are clicked, the Tax Payer data on the form will be used to update the Tax Payer in the database. This way, any edits will be captured</t>
-  </si>
-  <si>
-    <t>User enters Tax Return data as follows:
-*                                      Married filing jointly
-* Wages =                                        $ 95,000.00
-* Taxable Interest =                            1,242.16
-* Unemployment =                            1,115.53
-*                    Spouse claimed as Dependent
-* Withholding =                                10,628.38
-* Earned Income Credit =                         0.00
-* Nontaxable combat pay =                     0.00</t>
-  </si>
-  <si>
-    <t>User selects a tax year for which there is NOT a tax return in the database</t>
-  </si>
-  <si>
-    <t>User enters a tax year for which there IS a record in the database</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>Matthew Grayum</t>
-  </si>
-  <si>
-    <t>Professor Spiros Velianitis</t>
-  </si>
-  <si>
-    <t>Due Date: April 23, 2018</t>
-  </si>
-  <si>
-    <t>MIS 124 - Assignment 2</t>
-  </si>
-  <si>
-    <t>California State University Sacramento</t>
-  </si>
-  <si>
-    <t>Each test case was conducted to ensure that the application performed as expected</t>
-  </si>
-  <si>
-    <t>An error message will display, the DetailsView will remain in edit mode, and the record will not be updated</t>
-  </si>
-  <si>
-    <t>DetailsView edit mode: User enters an incorrectly formatted zip code</t>
-  </si>
-  <si>
-    <t>DetailsView edit mode: User enters an invalid State abbreviation</t>
+    <r>
+      <t xml:space="preserve">* Adjusted Grs Income =                                    $ 39,614.63
+* Standard Deduction =                                         10,400.00
+* Taxable Income =                                                29,214.63
+* Total Payments/Credits =                                     4,215.33
+* Tax =                                                                        3,918.00
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>* Amount of Refund =                                                297.33</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -525,7 +525,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -572,26 +572,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -936,8 +918,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A38FA25-0A53-450C-ACF4-C7A0D5762E98}">
   <dimension ref="A1:C38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -949,45 +931,45 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="7" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="7" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="7" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="7" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="8" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="B7" s="29"/>
-      <c r="C7" s="29"/>
+      <c r="A7" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="23"/>
+      <c r="C7" s="23"/>
     </row>
     <row r="8" spans="1:3" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="C8" s="1"/>
     </row>
     <row r="9" spans="1:3" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A9" s="26" t="s">
+      <c r="A9" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="27"/>
-      <c r="C9" s="28"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="22"/>
     </row>
     <row r="10" spans="1:3" s="2" customFormat="1" ht="29.1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A10" s="9" t="s">
@@ -1002,55 +984,55 @@
     </row>
     <row r="11" spans="1:3" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="10" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B11" s="12" t="s">
         <v>17</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="57.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="B12" s="30" t="s">
+      <c r="A12" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="20" t="s">
-        <v>42</v>
+      <c r="C12" s="16" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="31" t="s">
-        <v>50</v>
-      </c>
-      <c r="B13" s="30" t="s">
-        <v>49</v>
-      </c>
-      <c r="C13" s="20" t="s">
-        <v>42</v>
+      <c r="A13" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="29.1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A14" s="11" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
     <row r="16" spans="1:3" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A16" s="23" t="s">
+      <c r="A16" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="24"/>
-      <c r="C16" s="25"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="19"/>
     </row>
     <row r="17" spans="1:3" s="2" customFormat="1" ht="29.1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A17" s="4" t="s">
@@ -1064,171 +1046,171 @@
       </c>
     </row>
     <row r="18" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="17" t="s">
+      <c r="A18" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B18" s="18" t="s">
+      <c r="B18" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" s="16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" s="25"/>
+      <c r="B23" s="24"/>
+      <c r="C23" s="16"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" s="16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="C25" s="16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="C18" s="13" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="B19" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="C19" s="20" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="B20" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="C20" s="20" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="B21" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="C21" s="20" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="B22" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="C22" s="20" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="19"/>
-      <c r="B23" s="16"/>
-      <c r="C23" s="20"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="B24" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="C24" s="20" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25" s="19" t="s">
+      <c r="B26" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="C26" s="16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="C27" s="16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="B28" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28" s="16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="B29" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="C29" s="16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="B30" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" s="16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="B31" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="C31" s="16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="43.5" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A32" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B32" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="B25" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="C25" s="20" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="B26" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="C26" s="20" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="57.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="B27" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C27" s="20" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="B28" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="C28" s="20" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A29" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="B29" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="C29" s="20" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A30" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="B30" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="C30" s="20" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A31" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="B31" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="C31" s="20" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="43.5" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A32" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="B32" s="22" t="s">
-        <v>38</v>
-      </c>
       <c r="C32" s="15" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
     <row r="34" spans="1:3" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A34" s="23" t="s">
+      <c r="A34" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="B34" s="24"/>
-      <c r="C34" s="25"/>
+      <c r="B34" s="18"/>
+      <c r="C34" s="19"/>
     </row>
     <row r="35" spans="1:3" s="2" customFormat="1" ht="29.1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A35" s="4" t="s">
@@ -1242,36 +1224,36 @@
       </c>
     </row>
     <row r="36" spans="1:3" ht="129.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A36" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="B36" s="18" t="s">
-        <v>28</v>
+      <c r="A36" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B36" s="12" t="s">
+        <v>50</v>
       </c>
       <c r="C36" s="13" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="129.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A37" s="19" t="s">
+      <c r="A37" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="B37" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="C37" s="16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="29.1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A38" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="B37" s="16" t="s">
+      <c r="B38" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="C37" s="20" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="29.1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A38" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="B38" s="22" t="s">
-        <v>30</v>
-      </c>
       <c r="C38" s="15" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
successfuly displayed pie chart - added popup balloon on first page.
</commit_message>
<xml_diff>
--- a/Assignment_2/Assignment2_TestPlan/TestPlan.xlsx
+++ b/Assignment_2/Assignment2_TestPlan/TestPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthew Grayum\source\repos\MIS124\Assignment_2\Assignment2_TestPlan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65EBA726-3BCE-40F6-8E47-71682CAA5D5D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71F3043F-32E9-4F25-8AE6-33495148E2D6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14538" windowHeight="5886" xr2:uid="{00780A6C-A250-4A92-AB6B-E19A2F099472}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="53">
   <si>
     <t>Test Case</t>
   </si>
@@ -251,6 +251,9 @@
       </rPr>
       <t>* Amount of Refund =                                                297.33</t>
     </r>
+  </si>
+  <si>
+    <t>IEEE 829</t>
   </si>
 </sst>
 </file>
@@ -575,6 +578,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -595,12 +604,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -919,7 +922,7 @@
   <dimension ref="A1:C38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -933,6 +936,9 @@
       <c r="A1" s="7" t="s">
         <v>39</v>
       </c>
+      <c r="B1" s="1" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="7" t="s">
@@ -955,21 +961,21 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="23" t="s">
+      <c r="A7" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="B7" s="23"/>
-      <c r="C7" s="23"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="25"/>
     </row>
     <row r="8" spans="1:3" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="C8" s="1"/>
     </row>
     <row r="9" spans="1:3" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A9" s="20" t="s">
+      <c r="A9" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="21"/>
-      <c r="C9" s="22"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="24"/>
     </row>
     <row r="10" spans="1:3" s="2" customFormat="1" ht="29.1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A10" s="9" t="s">
@@ -994,10 +1000,10 @@
       </c>
     </row>
     <row r="12" spans="1:3" ht="57.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="25" t="s">
+      <c r="A12" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="24" t="s">
+      <c r="B12" s="17" t="s">
         <v>16</v>
       </c>
       <c r="C12" s="16" t="s">
@@ -1005,10 +1011,10 @@
       </c>
     </row>
     <row r="13" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="25" t="s">
+      <c r="A13" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="B13" s="24" t="s">
+      <c r="B13" s="17" t="s">
         <v>45</v>
       </c>
       <c r="C13" s="16" t="s">
@@ -1028,11 +1034,11 @@
     </row>
     <row r="15" spans="1:3" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
     <row r="16" spans="1:3" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A16" s="17" t="s">
+      <c r="A16" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="18"/>
-      <c r="C16" s="19"/>
+      <c r="B16" s="20"/>
+      <c r="C16" s="21"/>
     </row>
     <row r="17" spans="1:3" s="2" customFormat="1" ht="29.1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A17" s="4" t="s">
@@ -1057,10 +1063,10 @@
       </c>
     </row>
     <row r="19" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="25" t="s">
+      <c r="A19" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="B19" s="24" t="s">
+      <c r="B19" s="17" t="s">
         <v>29</v>
       </c>
       <c r="C19" s="16" t="s">
@@ -1068,10 +1074,10 @@
       </c>
     </row>
     <row r="20" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="25" t="s">
+      <c r="A20" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B20" s="24" t="s">
+      <c r="B20" s="17" t="s">
         <v>29</v>
       </c>
       <c r="C20" s="16" t="s">
@@ -1079,10 +1085,10 @@
       </c>
     </row>
     <row r="21" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="25" t="s">
+      <c r="A21" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="B21" s="24" t="s">
+      <c r="B21" s="17" t="s">
         <v>30</v>
       </c>
       <c r="C21" s="16" t="s">
@@ -1090,10 +1096,10 @@
       </c>
     </row>
     <row r="22" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" s="25" t="s">
+      <c r="A22" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B22" s="24" t="s">
+      <c r="B22" s="17" t="s">
         <v>30</v>
       </c>
       <c r="C22" s="16" t="s">
@@ -1101,15 +1107,15 @@
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="25"/>
-      <c r="B23" s="24"/>
+      <c r="A23" s="18"/>
+      <c r="B23" s="17"/>
       <c r="C23" s="16"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" s="25" t="s">
+      <c r="A24" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="B24" s="24" t="s">
+      <c r="B24" s="17" t="s">
         <v>8</v>
       </c>
       <c r="C24" s="16" t="s">
@@ -1117,10 +1123,10 @@
       </c>
     </row>
     <row r="25" spans="1:3" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25" s="25" t="s">
+      <c r="A25" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="B25" s="24" t="s">
+      <c r="B25" s="17" t="s">
         <v>21</v>
       </c>
       <c r="C25" s="16" t="s">
@@ -1128,10 +1134,10 @@
       </c>
     </row>
     <row r="26" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" s="25" t="s">
+      <c r="A26" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="B26" s="24" t="s">
+      <c r="B26" s="17" t="s">
         <v>20</v>
       </c>
       <c r="C26" s="16" t="s">
@@ -1139,10 +1145,10 @@
       </c>
     </row>
     <row r="27" spans="1:3" ht="57.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" s="25" t="s">
+      <c r="A27" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="B27" s="24" t="s">
+      <c r="B27" s="17" t="s">
         <v>23</v>
       </c>
       <c r="C27" s="16" t="s">
@@ -1150,10 +1156,10 @@
       </c>
     </row>
     <row r="28" spans="1:3" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28" s="25" t="s">
+      <c r="A28" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="B28" s="24" t="s">
+      <c r="B28" s="17" t="s">
         <v>10</v>
       </c>
       <c r="C28" s="16" t="s">
@@ -1161,10 +1167,10 @@
       </c>
     </row>
     <row r="29" spans="1:3" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A29" s="25" t="s">
+      <c r="A29" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="B29" s="24" t="s">
+      <c r="B29" s="17" t="s">
         <v>24</v>
       </c>
       <c r="C29" s="16" t="s">
@@ -1172,10 +1178,10 @@
       </c>
     </row>
     <row r="30" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A30" s="25" t="s">
+      <c r="A30" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="B30" s="24" t="s">
+      <c r="B30" s="17" t="s">
         <v>13</v>
       </c>
       <c r="C30" s="16" t="s">
@@ -1183,10 +1189,10 @@
       </c>
     </row>
     <row r="31" spans="1:3" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A31" s="25" t="s">
+      <c r="A31" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="B31" s="24" t="s">
+      <c r="B31" s="17" t="s">
         <v>15</v>
       </c>
       <c r="C31" s="16" t="s">
@@ -1206,11 +1212,11 @@
     </row>
     <row r="33" spans="1:3" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
     <row r="34" spans="1:3" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A34" s="17" t="s">
+      <c r="A34" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="B34" s="18"/>
-      <c r="C34" s="19"/>
+      <c r="B34" s="20"/>
+      <c r="C34" s="21"/>
     </row>
     <row r="35" spans="1:3" s="2" customFormat="1" ht="29.1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A35" s="4" t="s">
@@ -1235,10 +1241,10 @@
       </c>
     </row>
     <row r="37" spans="1:3" ht="129.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A37" s="25" t="s">
+      <c r="A37" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="B37" s="24" t="s">
+      <c r="B37" s="17" t="s">
         <v>51</v>
       </c>
       <c r="C37" s="16" t="s">

</xml_diff>